<commit_message>
new file with months not years
</commit_message>
<xml_diff>
--- a/resources/cashflow-challenge-example.xlsx
+++ b/resources/cashflow-challenge-example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dev\OneDrive\Documents\PeerIQ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{14758EF5-5718-4759-BC2D-09583A2C7755}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF059707-3DC4-4F0A-9C41-1FFE184430AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" xr2:uid="{7602C923-BD28-463E-A495-14F82BA54601}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" activeTab="1" xr2:uid="{7602C923-BD28-463E-A495-14F82BA54601}"/>
   </bookViews>
   <sheets>
     <sheet name="input" sheetId="1" r:id="rId1"/>
@@ -48,13 +48,7 @@
     <t>Interest Rate (APY)</t>
   </si>
   <si>
-    <t>Term (years)</t>
-  </si>
-  <si>
     <t>Welcome to the Cashflow Challenge Example Excel guide. As the readme indicates, this example computes the requested fields (in the output tab)</t>
-  </si>
-  <si>
-    <t>for a scenario with loan amount = $250,000; APY = 3.625%; and term = 30 years. Feel free to modify the input fields to check your</t>
   </si>
   <si>
     <t>work as well for the other scenarios! Good luck!</t>
@@ -79,6 +73,12 @@
   </si>
   <si>
     <t>total interest</t>
+  </si>
+  <si>
+    <t>Term (months)</t>
+  </si>
+  <si>
+    <t>for a scenario with loan amount = $250,000; APY = 3.625%; and term = 360 months (30 years). Feel free to modify the input fields to check your</t>
   </si>
 </sst>
 </file>
@@ -469,8 +469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62117E80-9449-42F2-9ACA-42F302C3804E}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -487,17 +487,17 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -513,7 +513,7 @@
         <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -524,7 +524,7 @@
         <v>3.6249999999999998E-2</v>
       </c>
       <c r="C9" s="4">
-        <v>30</v>
+        <v>360</v>
       </c>
     </row>
   </sheetData>
@@ -537,8 +537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{722974CA-BD08-4264-9097-8EE922985929}">
   <dimension ref="A1:G361"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -554,25 +554,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -584,7 +584,7 @@
         <v>250000</v>
       </c>
       <c r="C2" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D2" s="7">
@@ -613,7 +613,7 @@
         <v>249615.08007827791</v>
       </c>
       <c r="C3" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D3" s="7">
@@ -642,7 +642,7 @@
         <v>249228.99737762561</v>
       </c>
       <c r="C4" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D4" s="7">
@@ -671,7 +671,7 @@
         <v>248841.74838548174</v>
       </c>
       <c r="C5" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D5" s="7">
@@ -700,7 +700,7 @@
         <v>248453.32957867411</v>
       </c>
       <c r="C6" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D6" s="7">
@@ -729,7 +729,7 @@
         <v>248063.73742338759</v>
       </c>
       <c r="C7" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D7" s="7">
@@ -758,7 +758,7 @@
         <v>247672.96837513198</v>
       </c>
       <c r="C8" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D8" s="7">
@@ -787,7 +787,7 @@
         <v>247281.01887870976</v>
       </c>
       <c r="C9" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D9" s="7">
@@ -816,7 +816,7 @@
         <v>246887.88536818375</v>
       </c>
       <c r="C10" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D10" s="7">
@@ -845,7 +845,7 @@
         <v>246493.56426684471</v>
       </c>
       <c r="C11" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D11" s="7">
@@ -874,7 +874,7 @@
         <v>246098.05198717871</v>
       </c>
       <c r="C12" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D12" s="7">
@@ -903,7 +903,7 @@
         <v>245701.34493083454</v>
       </c>
       <c r="C13" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D13" s="7">
@@ -932,7 +932,7 @@
         <v>245303.43948859102</v>
       </c>
       <c r="C14" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D14" s="7">
@@ -961,7 +961,7 @@
         <v>244904.33204032402</v>
       </c>
       <c r="C15" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D15" s="7">
@@ -990,7 +990,7 @@
         <v>244504.01895497373</v>
       </c>
       <c r="C16" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D16" s="7">
@@ -1019,7 +1019,7 @@
         <v>244102.49659051144</v>
       </c>
       <c r="C17" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D17" s="7">
@@ -1048,7 +1048,7 @@
         <v>243699.76129390651</v>
       </c>
       <c r="C18" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D18" s="7">
@@ -1077,7 +1077,7 @@
         <v>243295.80940109308</v>
       </c>
       <c r="C19" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D19" s="7">
@@ -1106,7 +1106,7 @@
         <v>242890.63723693677</v>
       </c>
       <c r="C20" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D20" s="7">
@@ -1135,7 +1135,7 @@
         <v>242484.24111520126</v>
       </c>
       <c r="C21" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D21" s="7">
@@ -1164,7 +1164,7 @@
         <v>242076.61733851468</v>
       </c>
       <c r="C22" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D22" s="7">
@@ -1193,7 +1193,7 @@
         <v>241667.76219833601</v>
       </c>
       <c r="C23" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D23" s="7">
@@ -1222,7 +1222,7 @@
         <v>241257.6719749214</v>
       </c>
       <c r="C24" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D24" s="7">
@@ -1251,7 +1251,7 @@
         <v>240846.3429372902</v>
       </c>
       <c r="C25" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D25" s="7">
@@ -1280,7 +1280,7 @@
         <v>240433.77134319115</v>
       </c>
       <c r="C26" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D26" s="7">
@@ -1309,7 +1309,7 @@
         <v>240019.95343906828</v>
       </c>
       <c r="C27" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D27" s="7">
@@ -1338,7 +1338,7 @@
         <v>239604.88546002671</v>
       </c>
       <c r="C28" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D28" s="7">
@@ -1367,7 +1367,7 @@
         <v>239188.56362979845</v>
       </c>
       <c r="C29" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D29" s="7">
@@ -1396,7 +1396,7 @@
         <v>238770.98416070803</v>
       </c>
       <c r="C30" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D30" s="7">
@@ -1425,7 +1425,7 @@
         <v>238352.14325363806</v>
       </c>
       <c r="C31" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D31" s="7">
@@ -1454,7 +1454,7 @@
         <v>237932.03709799465</v>
       </c>
       <c r="C32" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D32" s="7">
@@ -1483,7 +1483,7 @@
         <v>237510.66187167272</v>
       </c>
       <c r="C33" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D33" s="7">
@@ -1512,7 +1512,7 @@
         <v>237088.01374102131</v>
       </c>
       <c r="C34" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D34" s="7">
@@ -1541,7 +1541,7 @@
         <v>236664.08886080855</v>
       </c>
       <c r="C35" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D35" s="7">
@@ -1570,7 +1570,7 @@
         <v>236238.88337418681</v>
       </c>
       <c r="C36" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D36" s="7">
@@ -1599,7 +1599,7 @@
         <v>235812.39341265758</v>
       </c>
       <c r="C37" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D37" s="7">
@@ -1628,7 +1628,7 @@
         <v>235384.61509603623</v>
       </c>
       <c r="C38" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D38" s="7">
@@ -1657,7 +1657,7 @@
         <v>234955.54453241674</v>
       </c>
       <c r="C39" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D39" s="7">
@@ -1686,7 +1686,7 @@
         <v>234525.17781813632</v>
       </c>
       <c r="C40" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D40" s="7">
@@ -1715,7 +1715,7 @@
         <v>234093.51103773984</v>
       </c>
       <c r="C41" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D41" s="7">
@@ -1744,7 +1744,7 @@
         <v>233660.54026394425</v>
       </c>
       <c r="C42" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D42" s="7">
@@ -1773,7 +1773,7 @@
         <v>233226.26155760282</v>
       </c>
       <c r="C43" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D43" s="7">
@@ -1802,7 +1802,7 @@
         <v>232790.67096766931</v>
       </c>
       <c r="C44" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D44" s="7">
@@ -1831,7 +1831,7 @@
         <v>232353.76453116204</v>
       </c>
       <c r="C45" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D45" s="7">
@@ -1860,7 +1860,7 @@
         <v>231915.53827312784</v>
       </c>
       <c r="C46" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D46" s="7">
@@ -1889,7 +1889,7 @@
         <v>231475.98820660581</v>
       </c>
       <c r="C47" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D47" s="7">
@@ -1918,7 +1918,7 @@
         <v>231035.11033259117</v>
       </c>
       <c r="C48" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D48" s="7">
@@ -1947,7 +1947,7 @@
         <v>230592.90063999878</v>
       </c>
       <c r="C49" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D49" s="7">
@@ -1976,7 +1976,7 @@
         <v>230149.35510562669</v>
       </c>
       <c r="C50" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D50" s="7">
@@ -2005,7 +2005,7 @@
         <v>229704.4696941195</v>
       </c>
       <c r="C51" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D51" s="7">
@@ -2034,7 +2034,7 @@
         <v>229258.24035793173</v>
       </c>
       <c r="C52" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D52" s="7">
@@ -2063,7 +2063,7 @@
         <v>228810.66303729088</v>
       </c>
       <c r="C53" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D53" s="7">
@@ -2092,7 +2092,7 @@
         <v>228361.73366016059</v>
       </c>
       <c r="C54" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D54" s="7">
@@ -2121,7 +2121,7 @@
         <v>227911.44814220356</v>
       </c>
       <c r="C55" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D55" s="7">
@@ -2150,7 +2150,7 @@
         <v>227459.80238674436</v>
       </c>
       <c r="C56" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D56" s="7">
@@ -2179,7 +2179,7 @@
         <v>227006.79228473222</v>
       </c>
       <c r="C57" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D57" s="7">
@@ -2208,7 +2208,7 @@
         <v>226552.41371470358</v>
       </c>
       <c r="C58" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D58" s="7">
@@ -2237,7 +2237,7 @@
         <v>226096.66254274466</v>
       </c>
       <c r="C59" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D59" s="7">
@@ -2266,7 +2266,7 @@
         <v>225639.53462245376</v>
       </c>
       <c r="C60" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D60" s="7">
@@ -2295,7 +2295,7 @@
         <v>225181.02579490366</v>
       </c>
       <c r="C61" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D61" s="7">
@@ -2324,7 +2324,7 @@
         <v>224721.13188860368</v>
       </c>
       <c r="C62" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D62" s="7">
@@ -2353,7 +2353,7 @@
         <v>224259.84871946173</v>
       </c>
       <c r="C63" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D63" s="7">
@@ -2382,7 +2382,7 @@
         <v>223797.17209074635</v>
       </c>
       <c r="C64" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D64" s="7">
@@ -2411,7 +2411,7 @@
         <v>223333.09779304836</v>
       </c>
       <c r="C65" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D65" s="7">
@@ -2440,7 +2440,7 @@
         <v>222867.62160424277</v>
       </c>
       <c r="C66" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D66" s="7">
@@ -2469,7 +2469,7 @@
         <v>222400.73928945017</v>
       </c>
       <c r="C67" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D67" s="7">
@@ -2498,7 +2498,7 @@
         <v>221932.44660099829</v>
       </c>
       <c r="C68" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D68" s="7">
@@ -2527,7 +2527,7 @@
         <v>221462.73927838338</v>
       </c>
       <c r="C69" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D69" s="7">
@@ -2556,7 +2556,7 @@
         <v>220991.6130482314</v>
       </c>
       <c r="C70" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D70" s="7">
@@ -2585,7 +2585,7 @@
         <v>220519.06362425917</v>
       </c>
       <c r="C71" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D71" s="7">
@@ -2614,7 +2614,7 @@
         <v>220045.08670723534</v>
       </c>
       <c r="C72" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D72" s="7">
@@ -2643,7 +2643,7 @@
         <v>219569.67798494134</v>
       </c>
       <c r="C73" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D73" s="7">
@@ -2672,7 +2672,7 @@
         <v>219092.8331321321</v>
       </c>
       <c r="C74" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D74" s="7">
@@ -2701,7 +2701,7 @@
         <v>218614.54781049665</v>
       </c>
       <c r="C75" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D75" s="7">
@@ -2730,7 +2730,7 @@
         <v>218134.81766861875</v>
       </c>
       <c r="C76" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D76" s="7">
@@ -2759,7 +2759,7 @@
         <v>217653.63834193727</v>
       </c>
       <c r="C77" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D77" s="7">
@@ -2788,7 +2788,7 @@
         <v>217171.00545270645</v>
       </c>
       <c r="C78" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D78" s="7">
@@ -2817,7 +2817,7 @@
         <v>216686.91460995606</v>
       </c>
       <c r="C79" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D79" s="7">
@@ -2846,7 +2846,7 @@
         <v>216201.36140945155</v>
       </c>
       <c r="C80" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D80" s="7">
@@ -2875,7 +2875,7 @@
         <v>215714.34143365384</v>
       </c>
       <c r="C81" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D81" s="7">
@@ -2904,7 +2904,7 @@
         <v>215225.85025167925</v>
       </c>
       <c r="C82" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D82" s="7">
@@ -2933,7 +2933,7 @@
         <v>214735.8834192591</v>
       </c>
       <c r="C83" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D83" s="7">
@@ -2962,7 +2962,7 @@
         <v>214244.43647869935</v>
       </c>
       <c r="C84" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D84" s="7">
@@ -2991,7 +2991,7 @@
         <v>213751.50495884</v>
       </c>
       <c r="C85" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D85" s="7">
@@ -3020,7 +3020,7 @@
         <v>213257.08437501438</v>
       </c>
       <c r="C86" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D86" s="7">
@@ -3049,7 +3049,7 @@
         <v>212761.17022900848</v>
       </c>
       <c r="C87" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D87" s="7">
@@ -3078,7 +3078,7 @@
         <v>212263.75800901983</v>
       </c>
       <c r="C88" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D88" s="7">
@@ -3107,7 +3107,7 @@
         <v>211764.84318961666</v>
       </c>
       <c r="C89" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D89" s="7">
@@ -3136,7 +3136,7 @@
         <v>211264.42123169653</v>
       </c>
       <c r="C90" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D90" s="7">
@@ -3165,7 +3165,7 @@
         <v>210762.48758244517</v>
       </c>
       <c r="C91" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D91" s="7">
@@ -3194,7 +3194,7 @@
         <v>210259.03767529505</v>
       </c>
       <c r="C92" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D92" s="7">
@@ -3223,7 +3223,7 @@
         <v>209754.06692988373</v>
       </c>
       <c r="C93" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D93" s="7">
@@ -3252,7 +3252,7 @@
         <v>209247.57075201231</v>
       </c>
       <c r="C94" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D94" s="7">
@@ -3281,7 +3281,7 @@
         <v>208739.54453360359</v>
       </c>
       <c r="C95" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D95" s="7">
@@ -3310,7 +3310,7 @@
         <v>208229.9836526601</v>
       </c>
       <c r="C96" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D96" s="7">
@@ -3339,7 +3339,7 @@
         <v>207718.88347322209</v>
       </c>
       <c r="C97" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D97" s="7">
@@ -3368,7 +3368,7 @@
         <v>207206.23934532533</v>
       </c>
       <c r="C98" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D98" s="7">
@@ -3397,7 +3397,7 @@
         <v>206692.04660495892</v>
       </c>
       <c r="C99" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D99" s="7">
@@ -3426,7 +3426,7 @@
         <v>206176.30057402264</v>
       </c>
       <c r="C100" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D100" s="7">
@@ -3455,7 +3455,7 @@
         <v>205658.99656028458</v>
       </c>
       <c r="C101" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D101" s="7">
@@ -3484,7 +3484,7 @@
         <v>205140.12985733832</v>
       </c>
       <c r="C102" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D102" s="7">
@@ -3513,7 +3513,7 @@
         <v>204619.69574456027</v>
       </c>
       <c r="C103" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D103" s="7">
@@ -3542,7 +3542,7 @@
         <v>204097.68948706653</v>
       </c>
       <c r="C104" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D104" s="7">
@@ -3571,7 +3571,7 @@
         <v>203574.10633566993</v>
       </c>
       <c r="C105" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D105" s="7">
@@ -3600,7 +3600,7 @@
         <v>203048.94152683683</v>
       </c>
       <c r="C106" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D106" s="7">
@@ -3629,7 +3629,7 @@
         <v>202522.19028264371</v>
       </c>
       <c r="C107" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D107" s="7">
@@ -3658,7 +3658,7 @@
         <v>201993.84781073377</v>
       </c>
       <c r="C108" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D108" s="7">
@@ -3687,7 +3687,7 @@
         <v>201463.90930427326</v>
       </c>
       <c r="C109" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D109" s="7">
@@ -3716,7 +3716,7 @@
         <v>200932.36994190782</v>
       </c>
       <c r="C110" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D110" s="7">
@@ -3745,7 +3745,7 @@
         <v>200399.22488771856</v>
       </c>
       <c r="C111" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D111" s="7">
@@ -3774,7 +3774,7 @@
         <v>199864.4692911781</v>
       </c>
       <c r="C112" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D112" s="7">
@@ -3803,7 +3803,7 @@
         <v>199328.09828710643</v>
       </c>
       <c r="C113" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D113" s="7">
@@ -3832,7 +3832,7 @@
         <v>198790.10699562664</v>
       </c>
       <c r="C114" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D114" s="7">
@@ -3861,7 +3861,7 @@
         <v>198250.4905221205</v>
       </c>
       <c r="C115" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D115" s="7">
@@ -3890,7 +3890,7 @@
         <v>197709.24395718396</v>
       </c>
       <c r="C116" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D116" s="7">
@@ -3919,7 +3919,7 @@
         <v>197166.36237658252</v>
       </c>
       <c r="C117" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D117" s="7">
@@ -3948,7 +3948,7 @@
         <v>196621.84084120634</v>
       </c>
       <c r="C118" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D118" s="7">
@@ -3977,7 +3977,7 @@
         <v>196075.6743970254</v>
       </c>
       <c r="C119" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D119" s="7">
@@ -4006,7 +4006,7 @@
         <v>195527.85807504432</v>
       </c>
       <c r="C120" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D120" s="7">
@@ -4035,7 +4035,7 @@
         <v>194978.38689125725</v>
       </c>
       <c r="C121" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D121" s="7">
@@ -4064,7 +4064,7 @@
         <v>194427.25584660249</v>
       </c>
       <c r="C122" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D122" s="7">
@@ -4093,7 +4093,7 @@
         <v>193874.45992691701</v>
       </c>
       <c r="C123" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D123" s="7">
@@ -4122,7 +4122,7 @@
         <v>193319.99410289081</v>
       </c>
       <c r="C124" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D124" s="7">
@@ -4151,7 +4151,7 @@
         <v>192763.8533300212</v>
       </c>
       <c r="C125" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D125" s="7">
@@ -4180,7 +4180,7 @@
         <v>192206.03254856687</v>
       </c>
       <c r="C126" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D126" s="7">
@@ -4209,7 +4209,7 @@
         <v>191646.5266835019</v>
       </c>
       <c r="C127" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D127" s="7">
@@ -4238,7 +4238,7 @@
         <v>191085.33064446953</v>
       </c>
       <c r="C128" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D128" s="7">
@@ -4267,7 +4267,7 @@
         <v>190522.43932573593</v>
       </c>
       <c r="C129" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D129" s="7">
@@ -4296,7 +4296,7 @@
         <v>189957.84760614365</v>
       </c>
       <c r="C130" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D130" s="7">
@@ -4325,7 +4325,7 @@
         <v>189391.5503490651</v>
       </c>
       <c r="C131" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D131" s="7">
@@ -4354,7 +4354,7 @@
         <v>188823.54240235582</v>
       </c>
       <c r="C132" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D132" s="7">
@@ -4383,7 +4383,7 @@
         <v>188253.81859830749</v>
       </c>
       <c r="C133" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D133" s="7">
@@ -4412,7 +4412,7 @@
         <v>187682.3737536011</v>
       </c>
       <c r="C134" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D134" s="7">
@@ -4441,7 +4441,7 @@
         <v>187109.20266925968</v>
       </c>
       <c r="C135" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D135" s="7">
@@ -4470,7 +4470,7 @@
         <v>186534.30013060098</v>
       </c>
       <c r="C136" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D136" s="7">
@@ -4499,7 +4499,7 @@
         <v>185957.66090719006</v>
       </c>
       <c r="C137" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D137" s="7">
@@ -4528,7 +4528,7 @@
         <v>185379.27975279177</v>
       </c>
       <c r="C138" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D138" s="7">
@@ -4557,7 +4557,7 @@
         <v>184799.15140532289</v>
       </c>
       <c r="C139" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D139" s="7">
@@ -4586,7 +4586,7 @@
         <v>184217.27058680437</v>
       </c>
       <c r="C140" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D140" s="7">
@@ -4615,7 +4615,7 @@
         <v>183633.63200331325</v>
       </c>
       <c r="C141" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D141" s="7">
@@ -4644,7 +4644,7 @@
         <v>183048.23034493451</v>
       </c>
       <c r="C142" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D142" s="7">
@@ -4673,7 +4673,7 @@
         <v>182461.06028571274</v>
       </c>
       <c r="C143" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D143" s="7">
@@ -4702,7 +4702,7 @@
         <v>181872.11648360372</v>
       </c>
       <c r="C144" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D144" s="7">
@@ -4731,7 +4731,7 @@
         <v>181281.39358042585</v>
       </c>
       <c r="C145" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D145" s="7">
@@ -4760,7 +4760,7 @@
         <v>180688.88620181128</v>
       </c>
       <c r="C146" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D146" s="7">
@@ -4789,7 +4789,7 @@
         <v>180094.58895715716</v>
       </c>
       <c r="C147" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D147" s="7">
@@ -4818,7 +4818,7 @@
         <v>179498.49643957647</v>
       </c>
       <c r="C148" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D148" s="7">
@@ -4847,7 +4847,7 @@
         <v>178900.60322584893</v>
       </c>
       <c r="C149" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D149" s="7">
@@ -4876,7 +4876,7 @@
         <v>178300.90387637159</v>
       </c>
       <c r="C150" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D150" s="7">
@@ -4905,7 +4905,7 @@
         <v>177699.39293510935</v>
       </c>
       <c r="C151" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D151" s="7">
@@ -4934,7 +4934,7 @@
         <v>177096.06492954539</v>
       </c>
       <c r="C152" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D152" s="7">
@@ -4963,7 +4963,7 @@
         <v>176490.9143706313</v>
       </c>
       <c r="C153" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D153" s="7">
@@ -4992,7 +4992,7 @@
         <v>175883.93575273716</v>
       </c>
       <c r="C154" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D154" s="7">
@@ -5021,7 +5021,7 @@
         <v>175275.12355360144</v>
       </c>
       <c r="C155" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D155" s="7">
@@ -5050,7 +5050,7 @@
         <v>174664.47223428084</v>
       </c>
       <c r="C156" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D156" s="7">
@@ -5079,7 +5079,7 @@
         <v>174051.97623909981</v>
       </c>
       <c r="C157" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D157" s="7">
@@ -5108,7 +5108,7 @@
         <v>173437.6299956</v>
       </c>
       <c r="C158" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D158" s="7">
@@ -5137,7 +5137,7 @@
         <v>172821.42791448961</v>
       </c>
       <c r="C159" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D159" s="7">
@@ -5166,7 +5166,7 @@
         <v>172203.36438959255</v>
       </c>
       <c r="C160" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D160" s="7">
@@ -5195,7 +5195,7 @@
         <v>171583.43379779733</v>
       </c>
       <c r="C161" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D161" s="7">
@@ -5224,7 +5224,7 @@
         <v>170961.63049900607</v>
       </c>
       <c r="C162" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D162" s="7">
@@ -5253,7 +5253,7 @@
         <v>170337.94883608306</v>
       </c>
       <c r="C163" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D163" s="7">
@@ -5282,7 +5282,7 @@
         <v>169712.3831348033</v>
       </c>
       <c r="C164" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D164" s="7">
@@ -5311,7 +5311,7 @@
         <v>169084.92770380093</v>
       </c>
       <c r="C165" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D165" s="7">
@@ -5340,7 +5340,7 @@
         <v>168455.57683451739</v>
       </c>
       <c r="C166" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D166" s="7">
@@ -5369,7 +5369,7 @@
         <v>167824.32480114955</v>
       </c>
       <c r="C167" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D167" s="7">
@@ -5398,7 +5398,7 @@
         <v>167191.1658605976</v>
       </c>
       <c r="C168" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D168" s="7">
@@ -5427,7 +5427,7 @@
         <v>166556.09425241273</v>
       </c>
       <c r="C169" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D169" s="7">
@@ -5456,7 +5456,7 @@
         <v>165919.10419874478</v>
       </c>
       <c r="C170" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D170" s="7">
@@ -5485,7 +5485,7 @@
         <v>165280.18990428973</v>
       </c>
       <c r="C171" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D171" s="7">
@@ -5514,7 +5514,7 @@
         <v>164639.34555623683</v>
       </c>
       <c r="C172" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D172" s="7">
@@ -5543,7 +5543,7 @@
         <v>163996.56532421586</v>
       </c>
       <c r="C173" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D173" s="7">
@@ -5572,7 +5572,7 @@
         <v>163351.84336024401</v>
       </c>
       <c r="C174" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D174" s="7">
@@ -5601,7 +5601,7 @@
         <v>162705.17379867265</v>
       </c>
       <c r="C175" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D175" s="7">
@@ -5630,7 +5630,7 @@
         <v>162056.55075613403</v>
       </c>
       <c r="C176" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D176" s="7">
@@ -5659,7 +5659,7 @@
         <v>161405.96833148776</v>
       </c>
       <c r="C177" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D177" s="7">
@@ -5688,7 +5688,7 @@
         <v>160753.42060576702</v>
       </c>
       <c r="C178" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D178" s="7">
@@ -5717,7 +5717,7 @@
         <v>160098.90164212484</v>
       </c>
       <c r="C179" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D179" s="7">
@@ -5746,7 +5746,7 @@
         <v>159442.40548577998</v>
       </c>
       <c r="C180" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D180" s="7">
@@ -5775,7 +5775,7 @@
         <v>158783.92616396284</v>
       </c>
       <c r="C181" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D181" s="7">
@@ -5804,7 +5804,7 @@
         <v>158123.45768586104</v>
       </c>
       <c r="C182" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D182" s="7">
@@ -5833,7 +5833,7 @@
         <v>157460.99404256497</v>
       </c>
       <c r="C183" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D183" s="7">
@@ -5862,7 +5862,7 @@
         <v>156796.52920701311</v>
       </c>
       <c r="C184" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D184" s="7">
@@ -5891,7 +5891,7 @@
         <v>156130.0571339372</v>
       </c>
       <c r="C185" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D185" s="7">
@@ -5920,7 +5920,7 @@
         <v>155461.57175980721</v>
       </c>
       <c r="C186" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D186" s="7">
@@ -5949,7 +5949,7 @@
         <v>154791.0670027762</v>
       </c>
       <c r="C187" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D187" s="7">
@@ -5978,7 +5978,7 @@
         <v>154118.53676262498</v>
       </c>
       <c r="C188" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D188" s="7">
@@ -6007,7 +6007,7 @@
         <v>153443.97492070665</v>
       </c>
       <c r="C189" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D189" s="7">
@@ -6036,7 +6036,7 @@
         <v>152767.37533989086</v>
       </c>
       <c r="C190" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D190" s="7">
@@ -6065,7 +6065,7 @@
         <v>152088.73186450801</v>
       </c>
       <c r="C191" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D191" s="7">
@@ -6094,7 +6094,7 @@
         <v>151408.03832029327</v>
       </c>
       <c r="C192" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D192" s="7">
@@ -6123,7 +6123,7 @@
         <v>150725.2885143304</v>
       </c>
       <c r="C193" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D193" s="7">
@@ -6152,7 +6152,7 @@
         <v>150040.47623499535</v>
       </c>
       <c r="C194" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D194" s="7">
@@ -6181,7 +6181,7 @@
         <v>149353.59525189979</v>
       </c>
       <c r="C195" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D195" s="7">
@@ -6210,7 +6210,7 @@
         <v>148664.63931583447</v>
       </c>
       <c r="C196" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D196" s="7">
@@ -6239,7 +6239,7 @@
         <v>147973.60215871228</v>
       </c>
       <c r="C197" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D197" s="7">
@@ -6268,7 +6268,7 @@
         <v>147280.47749351128</v>
       </c>
       <c r="C198" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D198" s="7">
@@ -6297,7 +6297,7 @@
         <v>146585.2590142175</v>
       </c>
       <c r="C199" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D199" s="7">
@@ -6326,7 +6326,7 @@
         <v>145887.94039576751</v>
       </c>
       <c r="C200" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D200" s="7">
@@ -6355,7 +6355,7 @@
         <v>145188.51529399096</v>
       </c>
       <c r="C201" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D201" s="7">
@@ -6384,7 +6384,7 @@
         <v>144486.97734555279</v>
       </c>
       <c r="C202" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D202" s="7">
@@ -6413,7 +6413,7 @@
         <v>143783.32016789538</v>
       </c>
       <c r="C203" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D203" s="7">
@@ -6442,7 +6442,7 @@
         <v>143077.53735918045</v>
       </c>
       <c r="C204" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D204" s="7">
@@ -6471,7 +6471,7 @@
         <v>142369.62249823089</v>
       </c>
       <c r="C205" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D205" s="7">
@@ -6500,7 +6500,7 @@
         <v>141659.56914447219</v>
       </c>
       <c r="C206" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D206" s="7">
@@ -6529,7 +6529,7 @@
         <v>140947.37083787401</v>
       </c>
       <c r="C207" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D207" s="7">
@@ -6558,7 +6558,7 @@
         <v>140233.02109889133</v>
       </c>
       <c r="C208" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D208" s="7">
@@ -6587,7 +6587,7 @@
         <v>139516.51342840548</v>
       </c>
       <c r="C209" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D209" s="7">
@@ -6616,7 +6616,7 @@
         <v>138797.84130766502</v>
       </c>
       <c r="C210" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D210" s="7">
@@ -6645,7 +6645,7 @@
         <v>138076.9981982265</v>
       </c>
       <c r="C211" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D211" s="7">
@@ -6674,7 +6674,7 @@
         <v>137353.97754189488</v>
       </c>
       <c r="C212" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D212" s="7">
@@ -6703,7 +6703,7 @@
         <v>136628.77276066394</v>
       </c>
       <c r="C213" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D213" s="7">
@@ -6732,7 +6732,7 @@
         <v>135901.37725665636</v>
       </c>
       <c r="C214" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D214" s="7">
@@ -6761,7 +6761,7 @@
         <v>135171.78441206375</v>
       </c>
       <c r="C215" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D215" s="7">
@@ -6790,7 +6790,7 @@
         <v>134439.98758908644</v>
       </c>
       <c r="C216" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D216" s="7">
@@ -6819,7 +6819,7 @@
         <v>133705.98012987303</v>
       </c>
       <c r="C217" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D217" s="7">
@@ -6848,7 +6848,7 @@
         <v>132969.75535645994</v>
       </c>
       <c r="C218" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D218" s="7">
@@ -6877,7 +6877,7 @@
         <v>132231.30657071047</v>
       </c>
       <c r="C219" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D219" s="7">
@@ -6906,7 +6906,7 @@
         <v>131490.62705425406</v>
       </c>
       <c r="C220" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D220" s="7">
@@ -6935,7 +6935,7 @@
         <v>130747.71006842502</v>
       </c>
       <c r="C221" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D221" s="7">
@@ -6964,7 +6964,7 @@
         <v>130002.54885420129</v>
       </c>
       <c r="C222" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D222" s="7">
@@ -6993,7 +6993,7 @@
         <v>129255.13663214292</v>
       </c>
       <c r="C223" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D223" s="7">
@@ -7022,7 +7022,7 @@
         <v>128505.46660233042</v>
       </c>
       <c r="C224" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D224" s="7">
@@ -7051,7 +7051,7 @@
         <v>127753.53194430286</v>
       </c>
       <c r="C225" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D225" s="7">
@@ -7080,7 +7080,7 @@
         <v>126999.32581699584</v>
       </c>
       <c r="C226" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D226" s="7">
@@ -7109,7 +7109,7 @@
         <v>126242.84135867924</v>
       </c>
       <c r="C227" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D227" s="7">
@@ -7138,7 +7138,7 @@
         <v>125484.07168689482</v>
       </c>
       <c r="C228" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D228" s="7">
@@ -7167,7 +7167,7 @@
         <v>124723.00989839355</v>
       </c>
       <c r="C229" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D229" s="7">
@@ -7196,7 +7196,7 @@
         <v>123959.64906907284</v>
       </c>
       <c r="C230" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D230" s="7">
@@ -7225,7 +7225,7 @@
         <v>123193.98225391356</v>
       </c>
       <c r="C231" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D231" s="7">
@@ -7254,7 +7254,7 @@
         <v>122426.00248691683</v>
       </c>
       <c r="C232" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D232" s="7">
@@ -7283,7 +7283,7 @@
         <v>121655.70278104063</v>
       </c>
       <c r="C233" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D233" s="7">
@@ -7312,7 +7312,7 @@
         <v>120883.07612813625</v>
       </c>
       <c r="C234" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D234" s="7">
@@ -7341,7 +7341,7 @@
         <v>120108.11549888457</v>
       </c>
       <c r="C235" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D235" s="7">
@@ -7370,7 +7370,7 @@
         <v>119330.81384273201</v>
       </c>
       <c r="C236" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D236" s="7">
@@ -7399,7 +7399,7 @@
         <v>118551.1640878265</v>
       </c>
       <c r="C237" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D237" s="7">
@@ -7428,7 +7428,7 @@
         <v>117769.15914095305</v>
       </c>
       <c r="C238" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D238" s="7">
@@ -7457,7 +7457,7 @@
         <v>116984.79188746926</v>
       </c>
       <c r="C239" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D239" s="7">
@@ -7486,7 +7486,7 @@
         <v>116198.05519124055</v>
       </c>
       <c r="C240" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D240" s="7">
@@ -7515,7 +7515,7 @@
         <v>115408.94189457533</v>
       </c>
       <c r="C241" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D241" s="7">
@@ -7544,7 +7544,7 @@
         <v>114617.44481815975</v>
       </c>
       <c r="C242" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D242" s="7">
@@ -7573,7 +7573,7 @@
         <v>113823.55676099252</v>
       </c>
       <c r="C243" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D243" s="7">
@@ -7602,7 +7602,7 @@
         <v>113027.27050031925</v>
       </c>
       <c r="C244" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D244" s="7">
@@ -7631,7 +7631,7 @@
         <v>112228.57879156686</v>
       </c>
       <c r="C245" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D245" s="7">
@@ -7660,7 +7660,7 @@
         <v>111427.47436827762</v>
       </c>
       <c r="C246" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D246" s="7">
@@ -7689,7 +7689,7 @@
         <v>110623.94994204302</v>
       </c>
       <c r="C247" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D247" s="7">
@@ -7718,7 +7718,7 @@
         <v>109817.99820243751</v>
       </c>
       <c r="C248" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D248" s="7">
@@ -7747,7 +7747,7 @@
         <v>109009.61181695193</v>
       </c>
       <c r="C249" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D249" s="7">
@@ -7776,7 +7776,7 @@
         <v>108198.78343092688</v>
       </c>
       <c r="C250" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D250" s="7">
@@ -7805,7 +7805,7 @@
         <v>107385.5056674857</v>
       </c>
       <c r="C251" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D251" s="7">
@@ -7834,7 +7834,7 @@
         <v>106569.77112746747</v>
       </c>
       <c r="C252" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D252" s="7">
@@ -7863,7 +7863,7 @@
         <v>105751.57238935959</v>
       </c>
       <c r="C253" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D253" s="7">
@@ -7892,7 +7892,7 @@
         <v>104930.90200923034</v>
       </c>
       <c r="C254" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D254" s="7">
@@ -7921,7 +7921,7 @@
         <v>104107.75252066112</v>
       </c>
       <c r="C255" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D255" s="7">
@@ -7950,7 +7950,7 @@
         <v>103282.11643467851</v>
       </c>
       <c r="C256" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D256" s="7">
@@ -7979,7 +7979,7 @@
         <v>102453.98623968617</v>
       </c>
       <c r="C257" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D257" s="7">
@@ -8008,7 +8008,7 @@
         <v>101623.35440139646</v>
       </c>
       <c r="C258" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D258" s="7">
@@ -8037,7 +8037,7 @@
         <v>100790.2133627619</v>
       </c>
       <c r="C259" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D259" s="7">
@@ -8066,7 +8066,7 @@
         <v>99954.555543906477</v>
       </c>
       <c r="C260" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D260" s="7">
@@ -8095,7 +8095,7 @@
         <v>99116.373342056599</v>
       </c>
       <c r="C261" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D261" s="7">
@@ -8124,7 +8124,7 @@
         <v>98275.659131471955</v>
       </c>
       <c r="C262" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D262" s="7">
@@ -8153,7 +8153,7 @@
         <v>97432.405263376175</v>
       </c>
       <c r="C263" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D263" s="7">
@@ -8182,7 +8182,7 @@
         <v>96586.604065887193</v>
       </c>
       <c r="C264" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D264" s="7">
@@ -8211,7 +8211,7 @@
         <v>95738.247843947465</v>
       </c>
       <c r="C265" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D265" s="7">
@@ -8240,7 +8240,7 @@
         <v>94887.328879253953</v>
       </c>
       <c r="C266" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D266" s="7">
@@ -8269,7 +8269,7 @@
         <v>94033.839430187931</v>
       </c>
       <c r="C267" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D267" s="7">
@@ -8298,7 +8298,7 @@
         <v>93177.77173174452</v>
       </c>
       <c r="C268" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D268" s="7">
@@ -8327,7 +8327,7 @@
         <v>92319.11799546206</v>
       </c>
       <c r="C269" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D269" s="7">
@@ -8356,7 +8356,7 @@
         <v>91457.87040935125</v>
       </c>
       <c r="C270" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D270" s="7">
@@ -8385,7 +8385,7 @@
         <v>90594.021137824064</v>
       </c>
       <c r="C271" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D271" s="7">
@@ -8414,7 +8414,7 @@
         <v>89727.562321622478</v>
       </c>
       <c r="C272" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D272" s="7">
@@ -8443,7 +8443,7 @@
         <v>88858.486077746944</v>
       </c>
       <c r="C273" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D273" s="7">
@@ -8472,7 +8472,7 @@
         <v>87986.78449938471</v>
       </c>
       <c r="C274" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D274" s="7">
@@ -8501,7 +8501,7 @@
         <v>87112.449655837831</v>
       </c>
       <c r="C275" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D275" s="7">
@@ -8530,7 +8530,7 @@
         <v>86235.473592451075</v>
       </c>
       <c r="C276" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D276" s="7">
@@ -8559,7 +8559,7 @@
         <v>85355.848330539506</v>
       </c>
       <c r="C277" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D277" s="7">
@@ -8588,7 +8588,7 @@
         <v>84473.565867315905</v>
       </c>
       <c r="C278" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D278" s="7">
@@ -8617,7 +8617,7 @@
         <v>83588.618175817988</v>
       </c>
       <c r="C279" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D279" s="7">
@@ -8646,7 +8646,7 @@
         <v>82700.997204835337</v>
       </c>
       <c r="C280" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D280" s="7">
@@ -8675,7 +8675,7 @@
         <v>81810.694878836177</v>
       </c>
       <c r="C281" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D281" s="7">
@@ -8704,7 +8704,7 @@
         <v>80917.7030978939</v>
       </c>
       <c r="C282" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D282" s="7">
@@ -8733,7 +8733,7 @@
         <v>80022.01373761335</v>
       </c>
       <c r="C283" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D283" s="7">
@@ -8762,7 +8762,7 @@
         <v>79123.618649056953</v>
       </c>
       <c r="C284" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D284" s="7">
@@ -8791,7 +8791,7 @@
         <v>78222.509658670548</v>
       </c>
       <c r="C285" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D285" s="7">
@@ -8820,7 +8820,7 @@
         <v>77318.678568209012</v>
       </c>
       <c r="C286" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D286" s="7">
@@ -8849,7 +8849,7 @@
         <v>76412.117154661712</v>
       </c>
       <c r="C287" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D287" s="7">
@@ -8878,7 +8878,7 @@
         <v>75502.817170177659</v>
       </c>
       <c r="C288" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D288" s="7">
@@ -8907,7 +8907,7 @@
         <v>74590.770341990472</v>
       </c>
       <c r="C289" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D289" s="7">
@@ -8936,7 +8936,7 @@
         <v>73675.968372343137</v>
       </c>
       <c r="C290" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D290" s="7">
@@ -8965,7 +8965,7 @@
         <v>72758.402938412488</v>
       </c>
       <c r="C291" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D291" s="7">
@@ -8994,7 +8994,7 @@
         <v>71838.065692233504</v>
       </c>
       <c r="C292" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D292" s="7">
@@ -9023,7 +9023,7 @@
         <v>70914.948260623365</v>
       </c>
       <c r="C293" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D293" s="7">
@@ -9052,7 +9052,7 @@
         <v>69989.042245105229</v>
       </c>
       <c r="C294" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D294" s="7">
@@ -9081,7 +9081,7 @@
         <v>69060.339221831891</v>
       </c>
       <c r="C295" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D295" s="7">
@@ -9110,7 +9110,7 @@
         <v>68128.830741509082</v>
       </c>
       <c r="C296" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D296" s="7">
@@ -9139,7 +9139,7 @@
         <v>67194.508329318618</v>
       </c>
       <c r="C297" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D297" s="7">
@@ -9168,7 +9168,7 @@
         <v>66257.363484841335</v>
       </c>
       <c r="C298" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D298" s="7">
@@ -9197,7 +9197,7 @@
         <v>65317.387681979693</v>
       </c>
       <c r="C299" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D299" s="7">
@@ -9226,7 +9226,7 @@
         <v>64374.572368880239</v>
       </c>
       <c r="C300" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D300" s="7">
@@ -9255,7 +9255,7 @@
         <v>63428.908967855801</v>
       </c>
       <c r="C301" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D301" s="7">
@@ -9284,7 +9284,7 @@
         <v>62480.388875307435</v>
       </c>
       <c r="C302" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D302" s="7">
@@ -9313,7 +9313,7 @@
         <v>61529.003461646163</v>
       </c>
       <c r="C303" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D303" s="7">
@@ -9342,7 +9342,7 @@
         <v>60574.744071214453</v>
       </c>
       <c r="C304" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D304" s="7">
@@ -9371,7 +9371,7 @@
         <v>59617.60202220748</v>
       </c>
       <c r="C305" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D305" s="7">
@@ -9400,7 +9400,7 @@
         <v>58657.568606594134</v>
       </c>
       <c r="C306" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D306" s="7">
@@ -9429,7 +9429,7 @@
         <v>57694.635090037787</v>
       </c>
       <c r="C307" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D307" s="7">
@@ -9458,7 +9458,7 @@
         <v>56728.792711816845</v>
       </c>
       <c r="C308" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D308" s="7">
@@ -9487,7 +9487,7 @@
         <v>55760.032684745027</v>
       </c>
       <c r="C309" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D309" s="7">
@@ -9516,7 +9516,7 @@
         <v>54788.346195091428</v>
       </c>
       <c r="C310" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D310" s="7">
@@ -9545,7 +9545,7 @@
         <v>53813.724402500331</v>
       </c>
       <c r="C311" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D311" s="7">
@@ -9574,7 +9574,7 @@
         <v>52836.158439910781</v>
       </c>
       <c r="C312" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D312" s="7">
@@ -9603,7 +9603,7 @@
         <v>51855.63941347591</v>
       </c>
       <c r="C313" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D313" s="7">
@@ -9632,7 +9632,7 @@
         <v>50872.158402482019</v>
       </c>
       <c r="C314" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D314" s="7">
@@ -9661,7 +9661,7 @@
         <v>49885.706459267414</v>
       </c>
       <c r="C315" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D315" s="7">
@@ -9690,7 +9690,7 @@
         <v>48896.274609141015</v>
       </c>
       <c r="C316" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D316" s="7">
@@ -9719,7 +9719,7 @@
         <v>47903.853850300693</v>
       </c>
       <c r="C317" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D317" s="7">
@@ -9748,7 +9748,7 @@
         <v>46908.435153751379</v>
       </c>
       <c r="C318" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D318" s="7">
@@ -9777,7 +9777,7 @@
         <v>45910.009463222901</v>
       </c>
       <c r="C319" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D319" s="7">
@@ -9806,7 +9806,7 @@
         <v>44908.567695087622</v>
       </c>
       <c r="C320" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D320" s="7">
@@ -9835,7 +9835,7 @@
         <v>43904.100738277768</v>
       </c>
       <c r="C321" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D321" s="7">
@@ -9864,7 +9864,7 @@
         <v>42896.599454202551</v>
       </c>
       <c r="C322" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D322" s="7">
@@ -9893,7 +9893,7 @@
         <v>41886.054676665022</v>
       </c>
       <c r="C323" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D323" s="7">
@@ -9922,7 +9922,7 @@
         <v>40872.457211778681</v>
       </c>
       <c r="C324" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D324" s="7">
@@ -9951,7 +9951,7 @@
         <v>39855.797837883831</v>
       </c>
       <c r="C325" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D325" s="7">
@@ -9980,7 +9980,7 @@
         <v>38836.067305463672</v>
       </c>
       <c r="C326" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D326" s="7">
@@ -10009,7 +10009,7 @@
         <v>37813.256337060164</v>
       </c>
       <c r="C327" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D327" s="7">
@@ -10038,7 +10038,7 @@
         <v>36787.355627189601</v>
       </c>
       <c r="C328" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D328" s="7">
@@ -10067,7 +10067,7 @@
         <v>35758.355842257974</v>
       </c>
       <c r="C329" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D329" s="7">
@@ -10096,7 +10096,7 @@
         <v>34726.247620476031</v>
       </c>
       <c r="C330" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D330" s="7">
@@ -10125,7 +10125,7 @@
         <v>33691.021571774123</v>
       </c>
       <c r="C331" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D331" s="7">
@@ -10154,7 +10154,7 @@
         <v>32652.668277716759</v>
       </c>
       <c r="C332" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D332" s="7">
@@ -10183,7 +10183,7 @@
         <v>31611.178291416931</v>
       </c>
       <c r="C333" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D333" s="7">
@@ -10212,7 +10212,7 @@
         <v>30566.542137450153</v>
       </c>
       <c r="C334" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D334" s="7">
@@ -10241,7 +10241,7 @@
         <v>29518.750311768268</v>
       </c>
       <c r="C335" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D335" s="7">
@@ -10270,7 +10270,7 @@
         <v>28467.793281612969</v>
       </c>
       <c r="C336" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D336" s="7">
@@ -10299,7 +10299,7 @@
         <v>27413.661485429075</v>
       </c>
       <c r="C337" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D337" s="7">
@@ -10328,7 +10328,7 @@
         <v>26356.345332777542</v>
       </c>
       <c r="C338" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D338" s="7">
@@ -10357,7 +10357,7 @@
         <v>25295.835204248207</v>
       </c>
       <c r="C339" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D339" s="7">
@@ -10386,7 +10386,7 @@
         <v>24232.121451372273</v>
       </c>
       <c r="C340" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D340" s="7">
@@ -10415,7 +10415,7 @@
         <v>23165.194396534527</v>
       </c>
       <c r="C341" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D341" s="7">
@@ -10444,7 +10444,7 @@
         <v>22095.044332885293</v>
       </c>
       <c r="C342" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D342" s="7">
@@ -10473,7 +10473,7 @@
         <v>21021.661524252118</v>
       </c>
       <c r="C343" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D343" s="7">
@@ -10502,7 +10502,7 @@
         <v>19945.036205051198</v>
       </c>
       <c r="C344" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D344" s="7">
@@ -10531,7 +10531,7 @@
         <v>18865.158580198524</v>
       </c>
       <c r="C345" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D345" s="7">
@@ -10560,7 +10560,7 @@
         <v>17782.018825020776</v>
       </c>
       <c r="C346" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D346" s="7">
@@ -10589,7 +10589,7 @@
         <v>16695.607085165928</v>
       </c>
       <c r="C347" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D347" s="7">
@@ -10618,7 +10618,7 @@
         <v>15605.9134765136</v>
       </c>
       <c r="C348" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D348" s="7">
@@ -10647,7 +10647,7 @@
         <v>14512.928085085136</v>
       </c>
       <c r="C349" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D349" s="7">
@@ -10676,7 +10676,7 @@
         <v>13416.640966953397</v>
       </c>
       <c r="C350" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D350" s="7">
@@ -10705,7 +10705,7 @@
         <v>12317.042148152303</v>
       </c>
       <c r="C351" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D351" s="7">
@@ -10734,7 +10734,7 @@
         <v>11214.12162458608</v>
       </c>
       <c r="C352" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D352" s="7">
@@ -10763,7 +10763,7 @@
         <v>10107.86936193825</v>
       </c>
       <c r="C353" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D353" s="7">
@@ -10792,7 +10792,7 @@
         <v>8998.2752955803389</v>
       </c>
       <c r="C354" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D354" s="7">
@@ -10821,7 +10821,7 @@
         <v>7885.3293304803055</v>
       </c>
       <c r="C355" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D355" s="7">
@@ -10850,7 +10850,7 @@
         <v>6769.0213411106988</v>
       </c>
       <c r="C356" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D356" s="7">
@@ -10879,7 +10879,7 @@
         <v>5649.3411713565383</v>
       </c>
       <c r="C357" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D357" s="7">
@@ -10908,7 +10908,7 @@
         <v>4526.2786344229116</v>
       </c>
       <c r="C358" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D358" s="7">
@@ -10937,7 +10937,7 @@
         <v>3399.8235127422986</v>
       </c>
       <c r="C359" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D359" s="7">
@@ -10966,7 +10966,7 @@
         <v>2269.9655578816082</v>
       </c>
       <c r="C360" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D360" s="7">
@@ -10995,7 +10995,7 @@
         <v>1136.6944904489433</v>
       </c>
       <c r="C361" s="8">
-        <f>PMT(input!$B$9/12,input!$C$9*12,input!$A$9)*-1</f>
+        <f>PMT(input!$B$9/12,input!$C$9,input!$A$9)*-1</f>
         <v>1140.1282550554324</v>
       </c>
       <c r="D361" s="7">

</xml_diff>